<commit_message>
Created test cases, in order to test our program. - Ethan
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-lab5-andrew_ethan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E955D01-8517-1C4D-BE7B-1C8D914E5AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F24F6D0-4034-4784-B7B3-E32DFB4ACB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -33,10 +33,122 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>Test Case Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Initial Balance</t>
+  </si>
+  <si>
+    <t>User Input</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>Valid Deposit</t>
+  </si>
+  <si>
+    <t>Valid Withdrawal</t>
+  </si>
+  <si>
+    <t>Withdraw more than balance</t>
+  </si>
+  <si>
+    <t>Negative Deposit</t>
+  </si>
+  <si>
+    <t>Negative Withdrawal</t>
+  </si>
+  <si>
+    <t>View Balance</t>
+  </si>
+  <si>
+    <t>Invalid Input</t>
+  </si>
+  <si>
+    <t>D, 200</t>
+  </si>
+  <si>
+    <t>W, 100</t>
+  </si>
+  <si>
+    <t>W, 1100</t>
+  </si>
+  <si>
+    <t>D, -100</t>
+  </si>
+  <si>
+    <t>W, -50</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Exit Program</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Balance: $1200.00</t>
+  </si>
+  <si>
+    <t>Balance: $900.00</t>
+  </si>
+  <si>
+    <t>Error: Insufficient funds.</t>
+  </si>
+  <si>
+    <t>Error: Cannot deposit a negative amount.</t>
+  </si>
+  <si>
+    <t>Error: Cannot withdraw a negative amount.</t>
+  </si>
+  <si>
+    <t>Balance: $1000.00</t>
+  </si>
+  <si>
+    <t>Error: Invalid choice.</t>
+  </si>
+  <si>
+    <t>"Thank you for using the ATM. Goodbye!"</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +176,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -124,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -230,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -372,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -380,14 +510,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{127005B9-9F5E-0446-B242-2658EACB013E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.125" customWidth="1"/>
+    <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="37.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>